<commit_message>
Fixed Send Email OTP
</commit_message>
<xml_diff>
--- a/src/components/Donation/LINS-Donations.xlsx
+++ b/src/components/Donation/LINS-Donations.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -516,9 +516,351 @@
         <v>11801</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>REC-1741876652886-252</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="str">
+        <v>2025-03-13T14:37:32.907Z</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E4" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F4" t="str">
+        <v>3445</v>
+      </c>
+      <c r="G4" t="str">
+        <v>dadhikari856@gmail.com</v>
+      </c>
+      <c r="H4" t="str">
+        <v>3477712375</v>
+      </c>
+      <c r="I4" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J4" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K4" t="str">
+        <v>NY</v>
+      </c>
+      <c r="L4" t="str">
+        <v>11801</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>REC-1741876747020-229</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="str">
+        <v>2025-03-13T14:39:07.031Z</v>
+      </c>
+      <c r="D5" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E5" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F5" t="str">
+        <v>3445</v>
+      </c>
+      <c r="G5" t="str">
+        <v>dadhikari856@gmail.com</v>
+      </c>
+      <c r="H5" t="str">
+        <v>3477712375</v>
+      </c>
+      <c r="I5" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J5" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K5" t="str">
+        <v>NY</v>
+      </c>
+      <c r="L5" t="str">
+        <v>11801</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>REC-1741876748126-582</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="str">
+        <v>2025-03-13T14:39:08.134Z</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E6" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F6" t="str">
+        <v>3445</v>
+      </c>
+      <c r="G6" t="str">
+        <v>dadhikari856@gmail.com</v>
+      </c>
+      <c r="H6" t="str">
+        <v>3477712375</v>
+      </c>
+      <c r="I6" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J6" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K6" t="str">
+        <v>NY</v>
+      </c>
+      <c r="L6" t="str">
+        <v>11801</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>REC-1741876748336-135</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="str">
+        <v>2025-03-13T14:39:08.338Z</v>
+      </c>
+      <c r="D7" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E7" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F7" t="str">
+        <v>3445</v>
+      </c>
+      <c r="G7" t="str">
+        <v>dadhikari856@gmail.com</v>
+      </c>
+      <c r="H7" t="str">
+        <v>3477712375</v>
+      </c>
+      <c r="I7" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J7" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K7" t="str">
+        <v>NY</v>
+      </c>
+      <c r="L7" t="str">
+        <v>11801</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>REC-1741876873473-419</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="str">
+        <v>2025-03-13T14:41:13.475Z</v>
+      </c>
+      <c r="D8" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E8" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F8" t="str">
+        <v>3445</v>
+      </c>
+      <c r="G8" t="str">
+        <v>dadhikari856@gmail.com</v>
+      </c>
+      <c r="H8" t="str">
+        <v>3477712375</v>
+      </c>
+      <c r="I8" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J8" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K8" t="str">
+        <v>NY</v>
+      </c>
+      <c r="L8" t="str">
+        <v>11801</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>REC-1741876962971-397</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="str">
+        <v>2025-03-13T14:42:42.973Z</v>
+      </c>
+      <c r="D9" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E9" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F9" t="str">
+        <v>3445</v>
+      </c>
+      <c r="G9" t="str">
+        <v>dadhikari856@gmail.com</v>
+      </c>
+      <c r="H9" t="str">
+        <v>3477712375</v>
+      </c>
+      <c r="I9" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J9" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K9" t="str">
+        <v>NY</v>
+      </c>
+      <c r="L9" t="str">
+        <v>11801</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>REC-1741876992736-933</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="str">
+        <v>2025-03-13T14:43:12.740Z</v>
+      </c>
+      <c r="D10" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E10" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F10" t="str">
+        <v>3445</v>
+      </c>
+      <c r="G10" t="str">
+        <v>dadhikari856@gmail.com</v>
+      </c>
+      <c r="H10" t="str">
+        <v>3477712375</v>
+      </c>
+      <c r="I10" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J10" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K10" t="str">
+        <v>NY</v>
+      </c>
+      <c r="L10" t="str">
+        <v>11801</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>REC-1741877009123-108</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="str">
+        <v>2025-03-13T14:43:29.132Z</v>
+      </c>
+      <c r="D11" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E11" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F11" t="str">
+        <v>3445</v>
+      </c>
+      <c r="G11" t="str">
+        <v>dadhikari856@gmail.com</v>
+      </c>
+      <c r="H11" t="str">
+        <v>3477712375</v>
+      </c>
+      <c r="I11" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J11" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K11" t="str">
+        <v>NY</v>
+      </c>
+      <c r="L11" t="str">
+        <v>11801</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>REC-1741877081275-061</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="str">
+        <v>2025-03-13T14:44:41.278Z</v>
+      </c>
+      <c r="D12" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E12" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F12" t="str">
+        <v>3445</v>
+      </c>
+      <c r="G12" t="str">
+        <v>dadhikari856@gmail.com</v>
+      </c>
+      <c r="H12" t="str">
+        <v>3477712375</v>
+      </c>
+      <c r="I12" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J12" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K12" t="str">
+        <v>NY</v>
+      </c>
+      <c r="L12" t="str">
+        <v>11801</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L12"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed Send Email OTP (#49)
Co-authored-by: SareePasal <sareepasalusa@gmail.com>
</commit_message>
<xml_diff>
--- a/src/components/Donation/LINS-Donations.xlsx
+++ b/src/components/Donation/LINS-Donations.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -516,9 +516,351 @@
         <v>11801</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>REC-1741876652886-252</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="str">
+        <v>2025-03-13T14:37:32.907Z</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E4" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F4" t="str">
+        <v>3445</v>
+      </c>
+      <c r="G4" t="str">
+        <v>dadhikari856@gmail.com</v>
+      </c>
+      <c r="H4" t="str">
+        <v>3477712375</v>
+      </c>
+      <c r="I4" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J4" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K4" t="str">
+        <v>NY</v>
+      </c>
+      <c r="L4" t="str">
+        <v>11801</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>REC-1741876747020-229</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="str">
+        <v>2025-03-13T14:39:07.031Z</v>
+      </c>
+      <c r="D5" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E5" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F5" t="str">
+        <v>3445</v>
+      </c>
+      <c r="G5" t="str">
+        <v>dadhikari856@gmail.com</v>
+      </c>
+      <c r="H5" t="str">
+        <v>3477712375</v>
+      </c>
+      <c r="I5" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J5" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K5" t="str">
+        <v>NY</v>
+      </c>
+      <c r="L5" t="str">
+        <v>11801</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>REC-1741876748126-582</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="str">
+        <v>2025-03-13T14:39:08.134Z</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E6" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F6" t="str">
+        <v>3445</v>
+      </c>
+      <c r="G6" t="str">
+        <v>dadhikari856@gmail.com</v>
+      </c>
+      <c r="H6" t="str">
+        <v>3477712375</v>
+      </c>
+      <c r="I6" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J6" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K6" t="str">
+        <v>NY</v>
+      </c>
+      <c r="L6" t="str">
+        <v>11801</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>REC-1741876748336-135</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="str">
+        <v>2025-03-13T14:39:08.338Z</v>
+      </c>
+      <c r="D7" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E7" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F7" t="str">
+        <v>3445</v>
+      </c>
+      <c r="G7" t="str">
+        <v>dadhikari856@gmail.com</v>
+      </c>
+      <c r="H7" t="str">
+        <v>3477712375</v>
+      </c>
+      <c r="I7" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J7" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K7" t="str">
+        <v>NY</v>
+      </c>
+      <c r="L7" t="str">
+        <v>11801</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>REC-1741876873473-419</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="str">
+        <v>2025-03-13T14:41:13.475Z</v>
+      </c>
+      <c r="D8" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E8" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F8" t="str">
+        <v>3445</v>
+      </c>
+      <c r="G8" t="str">
+        <v>dadhikari856@gmail.com</v>
+      </c>
+      <c r="H8" t="str">
+        <v>3477712375</v>
+      </c>
+      <c r="I8" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J8" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K8" t="str">
+        <v>NY</v>
+      </c>
+      <c r="L8" t="str">
+        <v>11801</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>REC-1741876962971-397</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="str">
+        <v>2025-03-13T14:42:42.973Z</v>
+      </c>
+      <c r="D9" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E9" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F9" t="str">
+        <v>3445</v>
+      </c>
+      <c r="G9" t="str">
+        <v>dadhikari856@gmail.com</v>
+      </c>
+      <c r="H9" t="str">
+        <v>3477712375</v>
+      </c>
+      <c r="I9" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J9" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K9" t="str">
+        <v>NY</v>
+      </c>
+      <c r="L9" t="str">
+        <v>11801</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>REC-1741876992736-933</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="str">
+        <v>2025-03-13T14:43:12.740Z</v>
+      </c>
+      <c r="D10" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E10" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F10" t="str">
+        <v>3445</v>
+      </c>
+      <c r="G10" t="str">
+        <v>dadhikari856@gmail.com</v>
+      </c>
+      <c r="H10" t="str">
+        <v>3477712375</v>
+      </c>
+      <c r="I10" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J10" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K10" t="str">
+        <v>NY</v>
+      </c>
+      <c r="L10" t="str">
+        <v>11801</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>REC-1741877009123-108</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="str">
+        <v>2025-03-13T14:43:29.132Z</v>
+      </c>
+      <c r="D11" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E11" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F11" t="str">
+        <v>3445</v>
+      </c>
+      <c r="G11" t="str">
+        <v>dadhikari856@gmail.com</v>
+      </c>
+      <c r="H11" t="str">
+        <v>3477712375</v>
+      </c>
+      <c r="I11" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J11" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K11" t="str">
+        <v>NY</v>
+      </c>
+      <c r="L11" t="str">
+        <v>11801</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>REC-1741877081275-061</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="str">
+        <v>2025-03-13T14:44:41.278Z</v>
+      </c>
+      <c r="D12" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E12" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F12" t="str">
+        <v>3445</v>
+      </c>
+      <c r="G12" t="str">
+        <v>dadhikari856@gmail.com</v>
+      </c>
+      <c r="H12" t="str">
+        <v>3477712375</v>
+      </c>
+      <c r="I12" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J12" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K12" t="str">
+        <v>NY</v>
+      </c>
+      <c r="L12" t="str">
+        <v>11801</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L12"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix ot pin prod (#50)
* Fixed Send Email OTP

* FizedOTPin PROD

---------

Co-authored-by: SareePasal <sareepasalusa@gmail.com>
</commit_message>
<xml_diff>
--- a/src/components/Donation/LINS-Donations.xlsx
+++ b/src/components/Donation/LINS-Donations.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -858,9 +858,85 @@
         <v>11801</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>REC-1741892275029-290</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="str">
+        <v>2025-03-13T18:57:55.037Z</v>
+      </c>
+      <c r="D13" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E13" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F13" t="str">
+        <v>123456</v>
+      </c>
+      <c r="G13" t="str">
+        <v>longislandnepalese@gmail.com</v>
+      </c>
+      <c r="H13" t="str">
+        <v>3477712375</v>
+      </c>
+      <c r="I13" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J13" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K13" t="str">
+        <v>NY</v>
+      </c>
+      <c r="L13" t="str">
+        <v>11801</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>REC-1741892978780-739</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" t="str">
+        <v>2025-03-13T19:09:38.787Z</v>
+      </c>
+      <c r="D14" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E14" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F14" t="str">
+        <v>2222</v>
+      </c>
+      <c r="G14" t="str">
+        <v>dadhikari856@gmail.com</v>
+      </c>
+      <c r="H14" t="str">
+        <v>3477712375</v>
+      </c>
+      <c r="I14" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J14" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K14" t="str">
+        <v>NY</v>
+      </c>
+      <c r="L14" t="str">
+        <v>11801</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L12"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L14"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Donation Page and Contact page
</commit_message>
<xml_diff>
--- a/src/components/Donation/LINS-Donations.xlsx
+++ b/src/components/Donation/LINS-Donations.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -439,6 +439,9 @@
       <c r="L1" t="str">
         <v>Zip</v>
       </c>
+      <c r="M1" t="str">
+        <v>PAID</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -934,9 +937,389 @@
         <v>11801</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>REC-1741969487529-984</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" t="str">
+        <v>2025-03-14T16:24:47.546Z</v>
+      </c>
+      <c r="D15" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E15" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F15" t="str">
+        <v>988</v>
+      </c>
+      <c r="G15" t="str">
+        <v>sjahbfkjadhkjfa@gmail.com</v>
+      </c>
+      <c r="H15" t="str">
+        <v>3477712375</v>
+      </c>
+      <c r="I15" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J15" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K15" t="str">
+        <v>NY</v>
+      </c>
+      <c r="L15" t="str">
+        <v>11801</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>REC-1741969570079-329</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16" t="str">
+        <v>2025-03-14T16:26:10.085Z</v>
+      </c>
+      <c r="D16" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E16" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F16" t="str">
+        <v>988</v>
+      </c>
+      <c r="G16" t="str">
+        <v>sjahbfkjadhkjfa@gmail.com</v>
+      </c>
+      <c r="H16" t="str">
+        <v>3477712375</v>
+      </c>
+      <c r="I16" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J16" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K16" t="str">
+        <v>NY</v>
+      </c>
+      <c r="L16" t="str">
+        <v>11801</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>REC-1741969650869-422</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17" t="str">
+        <v>2025-03-14T16:27:30.874Z</v>
+      </c>
+      <c r="D17" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E17" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F17" t="str">
+        <v>988</v>
+      </c>
+      <c r="G17" t="str">
+        <v>sjahbfkjadhkjfa@gmail.com</v>
+      </c>
+      <c r="H17" t="str">
+        <v>3477712375</v>
+      </c>
+      <c r="I17" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J17" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K17" t="str">
+        <v>NY</v>
+      </c>
+      <c r="L17" t="str">
+        <v>11801</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>REC-1741969739843-247</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18" t="str">
+        <v>2025-03-14T16:28:59.849Z</v>
+      </c>
+      <c r="D18" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E18" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F18" t="str">
+        <v>333333</v>
+      </c>
+      <c r="G18" t="str">
+        <v>dadhikari856@gmail.com</v>
+      </c>
+      <c r="H18" t="str">
+        <v>3477712375</v>
+      </c>
+      <c r="I18" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J18" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K18" t="str">
+        <v>NY</v>
+      </c>
+      <c r="L18" t="str">
+        <v>11801</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>REC-1741970623658-586</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19" t="str">
+        <v>2025-03-14T16:43:43.665Z</v>
+      </c>
+      <c r="D19" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E19" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F19" t="str">
+        <v>2222333</v>
+      </c>
+      <c r="G19" t="str">
+        <v>dadhikari856@gmail.com</v>
+      </c>
+      <c r="H19" t="str">
+        <v>3477712375</v>
+      </c>
+      <c r="I19" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J19" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K19" t="str">
+        <v>NY</v>
+      </c>
+      <c r="L19" t="str">
+        <v>11801</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>REC-1741970747227-173</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20" t="str">
+        <v>2025-03-14T16:45:47.232Z</v>
+      </c>
+      <c r="D20" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E20" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F20" t="str">
+        <v>2222333</v>
+      </c>
+      <c r="G20" t="str">
+        <v>dadhikari856@gmail.com</v>
+      </c>
+      <c r="H20" t="str">
+        <v>3477712375</v>
+      </c>
+      <c r="I20" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J20" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K20" t="str">
+        <v>NY</v>
+      </c>
+      <c r="L20" t="str">
+        <v>11801</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>REC-1741971092861-971</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" t="str">
+        <v>2025-03-14T16:51:32.867Z</v>
+      </c>
+      <c r="D21" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E21" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F21" t="str">
+        <v>2222333</v>
+      </c>
+      <c r="G21" t="str">
+        <v>dadhikari856@gmail.com</v>
+      </c>
+      <c r="H21" t="str">
+        <v>3477712375</v>
+      </c>
+      <c r="I21" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J21" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K21" t="str">
+        <v>NY</v>
+      </c>
+      <c r="L21" t="str">
+        <v>11801</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>REC-1741971120418-780</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22" t="str">
+        <v>2025-03-14T16:52:00.420Z</v>
+      </c>
+      <c r="D22" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E22" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F22" t="str">
+        <v>6666666666</v>
+      </c>
+      <c r="G22" t="str">
+        <v>dadhikari856@gmail.com</v>
+      </c>
+      <c r="H22" t="str">
+        <v>3477712375</v>
+      </c>
+      <c r="I22" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J22" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K22" t="str">
+        <v>NY</v>
+      </c>
+      <c r="L22" t="str">
+        <v>11801</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>REC-1741971739730-822</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23" t="str">
+        <v>2025-03-14T17:02:19.735Z</v>
+      </c>
+      <c r="D23" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E23" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F23" t="str">
+        <v>132</v>
+      </c>
+      <c r="G23" t="str">
+        <v>deepak-adhikari@hotmail.com</v>
+      </c>
+      <c r="H23" t="str">
+        <v>8567768105</v>
+      </c>
+      <c r="I23" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J23" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K23" t="str">
+        <v>Alabama</v>
+      </c>
+      <c r="L23" t="str">
+        <v>11801</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>REC-1741971785782-752</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24" t="str">
+        <v>2025-03-14T17:03:05.790Z</v>
+      </c>
+      <c r="D24" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E24" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F24" t="str">
+        <v>132</v>
+      </c>
+      <c r="G24" t="str">
+        <v>deepak-adhikari@taptap.com</v>
+      </c>
+      <c r="H24" t="str">
+        <v>8567768105</v>
+      </c>
+      <c r="I24" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J24" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K24" t="str">
+        <v>Alabama</v>
+      </c>
+      <c r="L24" t="str">
+        <v>11801</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L14"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M24"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Donation Page and Contact page (#54)
* Updated Donation Page and Contact page

* Adde subject line

---------

Co-authored-by: SareePasal <sareepasalusa@gmail.com>
</commit_message>
<xml_diff>
--- a/src/components/Donation/LINS-Donations.xlsx
+++ b/src/components/Donation/LINS-Donations.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -439,6 +439,9 @@
       <c r="L1" t="str">
         <v>Zip</v>
       </c>
+      <c r="M1" t="str">
+        <v>PAID</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -934,9 +937,389 @@
         <v>11801</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>REC-1741969487529-984</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" t="str">
+        <v>2025-03-14T16:24:47.546Z</v>
+      </c>
+      <c r="D15" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E15" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F15" t="str">
+        <v>988</v>
+      </c>
+      <c r="G15" t="str">
+        <v>sjahbfkjadhkjfa@gmail.com</v>
+      </c>
+      <c r="H15" t="str">
+        <v>3477712375</v>
+      </c>
+      <c r="I15" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J15" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K15" t="str">
+        <v>NY</v>
+      </c>
+      <c r="L15" t="str">
+        <v>11801</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>REC-1741969570079-329</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16" t="str">
+        <v>2025-03-14T16:26:10.085Z</v>
+      </c>
+      <c r="D16" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E16" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F16" t="str">
+        <v>988</v>
+      </c>
+      <c r="G16" t="str">
+        <v>sjahbfkjadhkjfa@gmail.com</v>
+      </c>
+      <c r="H16" t="str">
+        <v>3477712375</v>
+      </c>
+      <c r="I16" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J16" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K16" t="str">
+        <v>NY</v>
+      </c>
+      <c r="L16" t="str">
+        <v>11801</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>REC-1741969650869-422</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17" t="str">
+        <v>2025-03-14T16:27:30.874Z</v>
+      </c>
+      <c r="D17" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E17" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F17" t="str">
+        <v>988</v>
+      </c>
+      <c r="G17" t="str">
+        <v>sjahbfkjadhkjfa@gmail.com</v>
+      </c>
+      <c r="H17" t="str">
+        <v>3477712375</v>
+      </c>
+      <c r="I17" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J17" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K17" t="str">
+        <v>NY</v>
+      </c>
+      <c r="L17" t="str">
+        <v>11801</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>REC-1741969739843-247</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18" t="str">
+        <v>2025-03-14T16:28:59.849Z</v>
+      </c>
+      <c r="D18" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E18" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F18" t="str">
+        <v>333333</v>
+      </c>
+      <c r="G18" t="str">
+        <v>dadhikari856@gmail.com</v>
+      </c>
+      <c r="H18" t="str">
+        <v>3477712375</v>
+      </c>
+      <c r="I18" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J18" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K18" t="str">
+        <v>NY</v>
+      </c>
+      <c r="L18" t="str">
+        <v>11801</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>REC-1741970623658-586</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19" t="str">
+        <v>2025-03-14T16:43:43.665Z</v>
+      </c>
+      <c r="D19" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E19" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F19" t="str">
+        <v>2222333</v>
+      </c>
+      <c r="G19" t="str">
+        <v>dadhikari856@gmail.com</v>
+      </c>
+      <c r="H19" t="str">
+        <v>3477712375</v>
+      </c>
+      <c r="I19" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J19" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K19" t="str">
+        <v>NY</v>
+      </c>
+      <c r="L19" t="str">
+        <v>11801</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>REC-1741970747227-173</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20" t="str">
+        <v>2025-03-14T16:45:47.232Z</v>
+      </c>
+      <c r="D20" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E20" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F20" t="str">
+        <v>2222333</v>
+      </c>
+      <c r="G20" t="str">
+        <v>dadhikari856@gmail.com</v>
+      </c>
+      <c r="H20" t="str">
+        <v>3477712375</v>
+      </c>
+      <c r="I20" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J20" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K20" t="str">
+        <v>NY</v>
+      </c>
+      <c r="L20" t="str">
+        <v>11801</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>REC-1741971092861-971</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" t="str">
+        <v>2025-03-14T16:51:32.867Z</v>
+      </c>
+      <c r="D21" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E21" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F21" t="str">
+        <v>2222333</v>
+      </c>
+      <c r="G21" t="str">
+        <v>dadhikari856@gmail.com</v>
+      </c>
+      <c r="H21" t="str">
+        <v>3477712375</v>
+      </c>
+      <c r="I21" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J21" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K21" t="str">
+        <v>NY</v>
+      </c>
+      <c r="L21" t="str">
+        <v>11801</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>REC-1741971120418-780</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22" t="str">
+        <v>2025-03-14T16:52:00.420Z</v>
+      </c>
+      <c r="D22" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E22" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F22" t="str">
+        <v>6666666666</v>
+      </c>
+      <c r="G22" t="str">
+        <v>dadhikari856@gmail.com</v>
+      </c>
+      <c r="H22" t="str">
+        <v>3477712375</v>
+      </c>
+      <c r="I22" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J22" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K22" t="str">
+        <v>NY</v>
+      </c>
+      <c r="L22" t="str">
+        <v>11801</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>REC-1741971739730-822</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23" t="str">
+        <v>2025-03-14T17:02:19.735Z</v>
+      </c>
+      <c r="D23" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E23" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F23" t="str">
+        <v>132</v>
+      </c>
+      <c r="G23" t="str">
+        <v>deepak-adhikari@hotmail.com</v>
+      </c>
+      <c r="H23" t="str">
+        <v>8567768105</v>
+      </c>
+      <c r="I23" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J23" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K23" t="str">
+        <v>Alabama</v>
+      </c>
+      <c r="L23" t="str">
+        <v>11801</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>REC-1741971785782-752</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24" t="str">
+        <v>2025-03-14T17:03:05.790Z</v>
+      </c>
+      <c r="D24" t="str">
+        <v>Deepak</v>
+      </c>
+      <c r="E24" t="str">
+        <v>Adhikari</v>
+      </c>
+      <c r="F24" t="str">
+        <v>132</v>
+      </c>
+      <c r="G24" t="str">
+        <v>deepak-adhikari@taptap.com</v>
+      </c>
+      <c r="H24" t="str">
+        <v>8567768105</v>
+      </c>
+      <c r="I24" t="str">
+        <v>11 alpine ln</v>
+      </c>
+      <c r="J24" t="str">
+        <v>Hicksville</v>
+      </c>
+      <c r="K24" t="str">
+        <v>Alabama</v>
+      </c>
+      <c r="L24" t="str">
+        <v>11801</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L14"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M24"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>